<commit_message>
log, analysis and result for Wherewhenhownofoa_80_firstAttempt experiment
</commit_message>
<xml_diff>
--- a/Data/Result/Result_wherewhenhownofoa_80_firstAttempt.xlsx
+++ b/Data/Result/Result_wherewhenhownofoa_80_firstAttempt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\AL\Data\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14D56C0-A298-4B0A-9217-8737F7F7F299}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA603AF1-497C-48E7-8DBB-8C36EDFEB9F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24396" yWindow="312" windowWidth="21276" windowHeight="12744" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8448" yWindow="1488" windowWidth="16776" windowHeight="11964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem_type" sheetId="1" r:id="rId1"/>
@@ -2805,8 +2805,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3431,22 +3431,22 @@
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="10">
         <v>0.82</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="10">
         <v>0.82</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="10">
         <v>0.84</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="10">
         <v>0.86</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="10">
         <v>0.86</v>
       </c>
       <c r="H29" s="12"/>

</xml_diff>

<commit_message>
wherewhenhownofoa 80 first attempt result
</commit_message>
<xml_diff>
--- a/Data/Result/Result_wherewhenhownofoa_80_firstAttempt.xlsx
+++ b/Data/Result/Result_wherewhenhownofoa_80_firstAttempt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\AL\Data\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA603AF1-497C-48E7-8DBB-8C36EDFEB9F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C14CBDC-E87E-4B98-8135-695DE2D827EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8448" yWindow="1488" windowWidth="16776" windowHeight="11964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24300" yWindow="900" windowWidth="19512" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem_type" sheetId="1" r:id="rId1"/>
@@ -2361,16 +2361,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2705,8 +2705,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2805,8 +2805,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>